<commit_message>
rectify the fault in test case
</commit_message>
<xml_diff>
--- a/Question2/Dribble Testcases.xlsx
+++ b/Question2/Dribble Testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swost\OneDrive\Desktop\assessment-cloco\Question2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD269609-99D8-4DE4-8926-1F8003B7029A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF763038-5E9C-4B4C-AD7B-71E8A78B4318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2050,13 +2050,6 @@
     <t>User is on the "Create a New Collection" modal</t>
   </si>
   <si>
-    <t>1. Navigate to home page
-2. Select the product
-3. Click on "save shot" Icon
-4. Click on "Create a new colection" button
-5. Observe the create new coolection interface</t>
-  </si>
-  <si>
     <t>All elements should be visible and Presented.</t>
   </si>
   <si>
@@ -2089,11 +2082,6 @@
     <t>Verify the name field does not accept more than 64 characters.</t>
   </si>
   <si>
-    <t>1. Navigate to home page
-2. Enter a name with more than 64 characters
-3. Click "Create New Coolection" button</t>
-  </si>
-  <si>
     <t>More tha 65 characters</t>
   </si>
   <si>
@@ -2107,12 +2095,6 @@
   </si>
   <si>
     <t>Ensure the system does not allow an empty name</t>
-  </si>
-  <si>
-    <t>1. Navigate to home page
-2. Enter a name with more than 64 characters
-3. Leave name field empty and submit
-5. Click "Create New Coolection" button</t>
   </si>
   <si>
     <t>&lt;empty&gt;</t>
@@ -2648,6 +2630,24 @@
   <si>
     <t>User redirected to collections list page.</t>
   </si>
+  <si>
+    <t>1. Navigate to home page
+2. Enter a name with more than 64 characters
+3. Click "Create New Collection" button</t>
+  </si>
+  <si>
+    <t>1. Navigate to home page
+2. Select the product
+3. Click on "save shot" Icon
+4. Click on "Create a new collection" button
+5. Observe the create new collection interface</t>
+  </si>
+  <si>
+    <t>1. Navigate to home page
+2. Enter a name with more than 64 characters
+3. Leave name field empty and submit
+5. Click "Create New Collection" button</t>
+  </si>
 </sst>
 </file>
 
@@ -2777,7 +2777,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2796,6 +2796,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2809,7 +2815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2862,6 +2868,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2884,11 +2896,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3110,8 +3122,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="D27" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3289,10 +3301,10 @@
       <c r="AA5" s="3"/>
     </row>
     <row r="6" spans="1:27" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -3320,15 +3332,15 @@
       <c r="AA6" s="3"/>
     </row>
     <row r="7" spans="1:27" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -3422,7 +3434,7 @@
       <c r="H9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J9" s="3"/>
@@ -3469,7 +3481,7 @@
       <c r="H10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="I10" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J10" s="3"/>
@@ -3516,7 +3528,7 @@
       <c r="H11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J11" s="3"/>
@@ -3563,7 +3575,7 @@
       <c r="H12" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J12" s="3"/>
@@ -3610,7 +3622,7 @@
       <c r="H13" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J13" s="3"/>
@@ -3657,7 +3669,7 @@
       <c r="H14" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I14" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J14" s="3"/>
@@ -3709,17 +3721,17 @@
       <c r="AA15" s="3"/>
     </row>
     <row r="16" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -3811,7 +3823,7 @@
       <c r="H18" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I18" s="26" t="s">
+      <c r="I18" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J18" s="3"/>
@@ -3858,7 +3870,7 @@
       <c r="H19" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J19" s="3"/>
@@ -3905,7 +3917,7 @@
       <c r="H20" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="I20" s="26" t="s">
+      <c r="I20" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J20" s="3"/>
@@ -3952,7 +3964,7 @@
       <c r="H21" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I21" s="26" t="s">
+      <c r="I21" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J21" s="3"/>
@@ -3975,17 +3987,17 @@
       <c r="AA21" s="3"/>
     </row>
     <row r="22" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -4077,7 +4089,7 @@
       <c r="H24" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I24" s="26" t="s">
+      <c r="I24" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J24" s="3"/>
@@ -4124,7 +4136,7 @@
       <c r="H25" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="I25" s="26" t="s">
+      <c r="I25" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J25" s="3"/>
@@ -4171,7 +4183,7 @@
       <c r="H26" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="I26" s="26" t="s">
+      <c r="I26" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J26" s="3"/>
@@ -4218,7 +4230,7 @@
       <c r="H27" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I27" s="26" t="s">
+      <c r="I27" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J27" s="3"/>
@@ -4265,7 +4277,7 @@
       <c r="H28" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="I28" s="27" t="s">
+      <c r="I28" s="19" t="s">
         <v>124</v>
       </c>
       <c r="J28" s="3"/>
@@ -4312,7 +4324,7 @@
       <c r="H29" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="I29" s="27" t="s">
+      <c r="I29" s="19" t="s">
         <v>124</v>
       </c>
       <c r="J29" s="3"/>
@@ -4359,7 +4371,7 @@
       <c r="H30" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="I30" s="26" t="s">
+      <c r="I30" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J30" s="3"/>
@@ -4406,7 +4418,7 @@
       <c r="H31" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="I31" s="27" t="s">
+      <c r="I31" s="19" t="s">
         <v>124</v>
       </c>
       <c r="J31" s="3"/>
@@ -4453,7 +4465,7 @@
       <c r="H32" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="I32" s="27" t="s">
+      <c r="I32" s="19" t="s">
         <v>124</v>
       </c>
       <c r="J32" s="3"/>
@@ -4476,16 +4488,16 @@
       <c r="AA32" s="3"/>
     </row>
     <row r="33" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
       <c r="I33" s="6"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -4531,7 +4543,7 @@
       <c r="H34" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="I34" s="26" t="s">
+      <c r="I34" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J34" s="3"/>
@@ -4578,7 +4590,7 @@
       <c r="H35" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="I35" s="26" t="s">
+      <c r="I35" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J35" s="3"/>
@@ -4625,7 +4637,7 @@
       <c r="H36" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="I36" s="26" t="s">
+      <c r="I36" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J36" s="3"/>
@@ -4672,7 +4684,7 @@
       <c r="H37" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="I37" s="26" t="s">
+      <c r="I37" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J37" s="3"/>
@@ -4719,7 +4731,7 @@
       <c r="H38" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="I38" s="26" t="s">
+      <c r="I38" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J38" s="3"/>
@@ -4742,16 +4754,16 @@
       <c r="AA38" s="3"/>
     </row>
     <row r="39" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -4797,7 +4809,7 @@
       <c r="H40" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="I40" s="26" t="s">
+      <c r="I40" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J40" s="3"/>
@@ -4844,7 +4856,7 @@
       <c r="H41" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="I41" s="26" t="s">
+      <c r="I41" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J41" s="3"/>
@@ -4891,7 +4903,7 @@
       <c r="H42" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="I42" s="26" t="s">
+      <c r="I42" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J42" s="3"/>
@@ -4938,7 +4950,7 @@
       <c r="H43" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="I43" s="27" t="s">
+      <c r="I43" s="19" t="s">
         <v>124</v>
       </c>
       <c r="J43" s="3"/>
@@ -4985,7 +4997,7 @@
       <c r="H44" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="I44" s="26" t="s">
+      <c r="I44" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J44" s="3"/>
@@ -5032,7 +5044,7 @@
       <c r="H45" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="I45" s="26" t="s">
+      <c r="I45" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J45" s="3"/>
@@ -5079,7 +5091,7 @@
       <c r="H46" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="I46" s="26" t="s">
+      <c r="I46" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J46" s="3"/>
@@ -5126,7 +5138,7 @@
       <c r="H47" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="I47" s="26" t="s">
+      <c r="I47" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J47" s="3"/>
@@ -5173,7 +5185,7 @@
       <c r="H48" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="I48" s="26" t="s">
+      <c r="I48" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J48" s="3"/>
@@ -5220,7 +5232,7 @@
       <c r="H49" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="I49" s="26" t="s">
+      <c r="I49" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J49" s="3"/>
@@ -5243,15 +5255,15 @@
       <c r="AA49" s="3"/>
     </row>
     <row r="50" spans="1:27" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
       <c r="H50" s="3"/>
       <c r="I50" s="6"/>
       <c r="J50" s="3"/>
@@ -5298,7 +5310,7 @@
       <c r="H51" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="I51" s="26" t="s">
+      <c r="I51" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J51" s="3"/>
@@ -5345,7 +5357,7 @@
       <c r="H52" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="I52" s="26" t="s">
+      <c r="I52" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J52" s="3"/>
@@ -5392,7 +5404,7 @@
       <c r="H53" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="I53" s="26" t="s">
+      <c r="I53" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J53" s="3"/>
@@ -5439,7 +5451,7 @@
       <c r="H54" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="I54" s="26" t="s">
+      <c r="I54" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J54" s="3"/>
@@ -5462,15 +5474,15 @@
       <c r="AA54" s="3"/>
     </row>
     <row r="55" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
@@ -5517,7 +5529,7 @@
       <c r="H56" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="I56" s="26" t="s">
+      <c r="I56" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J56" s="3"/>
@@ -5564,7 +5576,7 @@
       <c r="H57" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="I57" s="26" t="s">
+      <c r="I57" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J57" s="3"/>
@@ -5587,15 +5599,15 @@
       <c r="AA57" s="3"/>
     </row>
     <row r="58" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="18" t="s">
+      <c r="A58" s="20" t="s">
         <v>298</v>
       </c>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
@@ -5642,7 +5654,7 @@
       <c r="H59" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="I59" s="26" t="s">
+      <c r="I59" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J59" s="3"/>
@@ -5689,7 +5701,7 @@
       <c r="H60" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="I60" s="26" t="s">
+      <c r="I60" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J60" s="3"/>
@@ -5736,7 +5748,7 @@
       <c r="H61" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="I61" s="26" t="s">
+      <c r="I61" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J61" s="3"/>
@@ -5783,7 +5795,7 @@
       <c r="H62" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="I62" s="26" t="s">
+      <c r="I62" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J62" s="3"/>
@@ -5806,15 +5818,15 @@
       <c r="AA62" s="3"/>
     </row>
     <row r="63" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="18" t="s">
+      <c r="A63" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B63" s="19"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
@@ -5861,7 +5873,7 @@
       <c r="H64" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="I64" s="26" t="s">
+      <c r="I64" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J64" s="3"/>
@@ -33062,7 +33074,9 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33151,10 +33165,10 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -33164,15 +33178,15 @@
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
@@ -33230,7 +33244,7 @@
       <c r="H9" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33259,7 +33273,7 @@
       <c r="H10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33288,7 +33302,7 @@
       <c r="H11" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33317,7 +33331,7 @@
       <c r="H12" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33346,7 +33360,7 @@
       <c r="H13" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33375,7 +33389,7 @@
       <c r="H14" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33404,20 +33418,20 @@
       <c r="H15" s="9" t="s">
         <v>377</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="19" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="26" t="s">
         <v>378</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
     </row>
@@ -33446,7 +33460,7 @@
       <c r="H17" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33475,7 +33489,7 @@
       <c r="H18" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33504,7 +33518,7 @@
       <c r="H19" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33533,7 +33547,7 @@
       <c r="H20" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33562,7 +33576,7 @@
       <c r="H21" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33591,7 +33605,7 @@
       <c r="H22" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="19" t="s">
         <v>124</v>
       </c>
     </row>
@@ -33620,7 +33634,7 @@
       <c r="H23" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="19" t="s">
         <v>124</v>
       </c>
     </row>
@@ -33649,7 +33663,7 @@
       <c r="H24" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -33678,7 +33692,7 @@
       <c r="H25" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -44432,7 +44446,9 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -44520,10 +44536,10 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -44533,15 +44549,15 @@
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="20" t="s">
         <v>438</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
@@ -44599,7 +44615,7 @@
       <c r="H9" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -44628,7 +44644,7 @@
       <c r="H10" s="9" t="s">
         <v>451</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -44657,7 +44673,7 @@
       <c r="H11" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -44686,22 +44702,22 @@
       <c r="H12" s="9" t="s">
         <v>463</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="26" t="s">
         <v>464</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="6"/>
+      <c r="I13" s="28"/>
     </row>
     <row r="14" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -44728,7 +44744,7 @@
       <c r="H14" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -44757,7 +44773,7 @@
       <c r="H15" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="19" t="s">
         <v>124</v>
       </c>
     </row>
@@ -44786,7 +44802,7 @@
       <c r="H16" s="9" t="s">
         <v>485</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="19" t="s">
         <v>124</v>
       </c>
     </row>
@@ -44815,7 +44831,7 @@
       <c r="H17" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -44844,7 +44860,7 @@
       <c r="H18" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -44873,7 +44889,7 @@
       <c r="H19" s="9" t="s">
         <v>504</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="19" t="s">
         <v>124</v>
       </c>
     </row>
@@ -44902,7 +44918,7 @@
       <c r="H20" s="9" t="s">
         <v>511</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="19" t="s">
         <v>124</v>
       </c>
     </row>
@@ -44931,7 +44947,7 @@
       <c r="H21" s="9" t="s">
         <v>518</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -55729,11 +55745,13 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
     <col min="2" max="2" width="28.21875" customWidth="1"/>
     <col min="3" max="3" width="29.77734375" customWidth="1"/>
     <col min="4" max="4" width="28.88671875" customWidth="1"/>
@@ -55743,7 +55761,7 @@
     <col min="8" max="8" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -55773,7 +55791,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
@@ -55788,7 +55806,7 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -55803,7 +55821,7 @@
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
@@ -55816,11 +55834,11 @@
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -55830,15 +55848,15 @@
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
@@ -55885,18 +55903,18 @@
         <v>523</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>524</v>
+        <v>644</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>526</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -55905,27 +55923,27 @@
         <v>28</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>527</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>528</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>523</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="G10" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>531</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>532</v>
-      </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -55934,27 +55952,27 @@
         <v>34</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>533</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>534</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>523</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>535</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="H11" s="9" t="s">
         <v>536</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>537</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>538</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -55963,27 +55981,27 @@
         <v>40</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>523</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>541</v>
+        <v>645</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>396</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>543</v>
-      </c>
-      <c r="I12" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="I12" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -55992,27 +56010,27 @@
         <v>46</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>523</v>
       </c>
       <c r="E13" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>544</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>546</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>547</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>548</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>549</v>
-      </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -56021,430 +56039,430 @@
         <v>53</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>523</v>
       </c>
       <c r="E14" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>552</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>553</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>554</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>555</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>523</v>
       </c>
       <c r="E15" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>557</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>559</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>560</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>562</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>523</v>
       </c>
       <c r="E16" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>566</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>567</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>568</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>569</v>
-      </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>523</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>575</v>
-      </c>
-      <c r="I17" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="I17" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>523</v>
       </c>
       <c r="E18" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>579</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>580</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>581</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>582</v>
-      </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="19" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>583</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>584</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="F19" s="8" t="s">
         <v>585</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="G19" s="9" t="s">
         <v>586</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="H19" s="9" t="s">
         <v>587</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="I19" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
         <v>588</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>590</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>591</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>592</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="E21" s="9" t="s">
         <v>593</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="F21" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="H21" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>597</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>598</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>599</v>
-      </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>600</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>601</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="G22" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>602</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>595</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>603</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>604</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>537</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>605</v>
-      </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>604</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>606</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>540</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>595</v>
-      </c>
-      <c r="E23" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>607</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>608</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>609</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>610</v>
-      </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="F24" s="8" t="s">
         <v>612</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>595</v>
-      </c>
-      <c r="E24" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>614</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>615</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>616</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>617</v>
-      </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>617</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>618</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>619</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>620</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>595</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>621</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>24</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="I25" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="I25" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>624</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+      <c r="A26" s="20" t="s">
+        <v>621</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
       <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
+      <c r="I26" s="29"/>
     </row>
     <row r="27" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>625</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="E27" s="9" t="s">
         <v>626</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>627</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>628</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>629</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>24</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>631</v>
-      </c>
-      <c r="I27" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="I27" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>632</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="E28" s="9" t="s">
         <v>633</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>634</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>635</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>636</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>24</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>638</v>
-      </c>
-      <c r="I28" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="I28" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>639</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="E29" s="9" t="s">
         <v>640</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>641</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>643</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>24</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>645</v>
-      </c>
-      <c r="I29" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="I29" s="28" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>